<commit_message>
Analysis on non-linear relationships
</commit_message>
<xml_diff>
--- a/RAW/Variables_Listing_V2.xlsx
+++ b/RAW/Variables_Listing_V2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="719"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="719" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Property Price" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Price Services" sheetId="6" r:id="rId5"/>
     <sheet name="Additional feat" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="108">
   <si>
     <t>LotFrontage</t>
   </si>
@@ -369,12 +369,21 @@
   <si>
     <t>top30</t>
   </si>
+  <si>
+    <t>Costly material and more area would mean more money</t>
+  </si>
+  <si>
+    <t>Using 2 materials on the surface would be more expensive; also costly materials would mean more money</t>
+  </si>
+  <si>
+    <t>Get the total number of finishes used</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,14 +405,6 @@
       <family val="3"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
       <color theme="1"/>
@@ -419,7 +420,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +451,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -463,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -473,16 +492,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -888,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1020,7 @@
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="11"/>
       <c r="D10" t="s">
         <v>100</v>
       </c>
@@ -1006,7 +1035,7 @@
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>99</v>
       </c>
       <c r="E11" t="s">
@@ -1058,6 +1087,9 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C16" s="14" t="s">
+        <v>107</v>
+      </c>
       <c r="E16" t="s">
         <v>102</v>
       </c>
@@ -1069,6 +1101,7 @@
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -1091,25 +1124,33 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="34.5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -1120,7 +1161,7 @@
       <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="8" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1128,12 +1169,16 @@
       <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="8" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C16:C17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1142,7 +1187,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,7 +1220,7 @@
       <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>96</v>
       </c>
       <c r="E3" t="s">
@@ -1282,7 +1327,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1525,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1550,7 @@
       <c r="B3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1522,7 +1567,7 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1530,13 +1575,13 @@
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -1548,7 +1593,7 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="10"/>
       <c r="D10" t="s">
         <v>100</v>
       </c>
@@ -1563,7 +1608,7 @@
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="11"/>
       <c r="D11" t="s">
         <v>100</v>
       </c>

</xml_diff>